<commit_message>
Ajustes na validacao do df e tipos do consolidado. Criacao do Raise no Validar, se falhar, tabela não é criada! Passou tudo, validadooo
</commit_message>
<xml_diff>
--- a/data/processed/vendas.xlsx
+++ b/data/processed/vendas.xlsx
@@ -471,15 +471,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A2" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -506,15 +502,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -541,15 +533,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A4" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -576,15 +564,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -611,15 +595,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -646,15 +626,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A7" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -681,15 +657,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A8" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -716,15 +688,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A9" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -751,15 +719,11 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A10" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B10" t="n">
+        <v>6</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -786,15 +750,11 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -821,15 +781,11 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A12" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -856,15 +812,11 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A13" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B13" t="n">
+        <v>7</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -891,15 +843,11 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A14" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B14" t="n">
+        <v>8</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -926,15 +874,11 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -961,15 +905,11 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A16" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -996,15 +936,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A17" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1031,15 +967,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A18" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1066,15 +998,11 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A19" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B19" t="n">
+        <v>8</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1101,15 +1029,11 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A20" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1136,15 +1060,11 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A21" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1171,15 +1091,11 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A22" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1206,15 +1122,11 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A23" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B23" t="n">
+        <v>6</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1241,15 +1153,11 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A24" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B24" t="n">
+        <v>4</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1276,15 +1184,11 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A25" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B25" t="n">
+        <v>7</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1311,15 +1215,11 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A26" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B26" t="n">
+        <v>3</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1346,15 +1246,11 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A27" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B27" t="n">
+        <v>5</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1381,15 +1277,11 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A28" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B28" t="n">
+        <v>7</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1416,15 +1308,11 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A29" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1451,15 +1339,11 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A30" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B30" t="n">
+        <v>6</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1486,15 +1370,11 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A31" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1521,15 +1401,11 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A32" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B32" t="n">
+        <v>4</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1556,15 +1432,11 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A33" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B33" t="n">
+        <v>8</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1591,15 +1463,11 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A34" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B34" t="n">
+        <v>7</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1626,15 +1494,11 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A35" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B35" t="n">
+        <v>8</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1661,15 +1525,11 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A36" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1696,15 +1556,11 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A37" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B37" t="n">
+        <v>5</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1731,15 +1587,11 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A38" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B38" t="n">
+        <v>6</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1766,15 +1618,11 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A39" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B39" t="n">
+        <v>3</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1801,15 +1649,11 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A40" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1836,15 +1680,11 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A41" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B41" t="n">
+        <v>4</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1871,15 +1711,11 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A42" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B42" t="n">
+        <v>4</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1906,15 +1742,11 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A43" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B43" t="n">
+        <v>6</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1941,15 +1773,11 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A44" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B44" t="n">
+        <v>7</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1976,15 +1804,11 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A45" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B45" t="n">
+        <v>2</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2011,15 +1835,11 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A46" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2046,15 +1866,11 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A47" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2081,15 +1897,11 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A48" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B48" t="n">
+        <v>5</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2116,15 +1928,11 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A49" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B49" t="n">
+        <v>8</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2151,15 +1959,11 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A50" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B50" t="n">
+        <v>6</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2186,15 +1990,11 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A51" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B51" t="n">
+        <v>5</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2221,15 +2021,11 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A52" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B52" t="n">
+        <v>7</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2256,15 +2052,11 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A53" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2291,15 +2083,11 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A54" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B54" t="n">
+        <v>8</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2326,15 +2114,11 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A55" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B55" t="n">
+        <v>4</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2361,15 +2145,11 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A56" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -2396,15 +2176,11 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A57" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -2431,15 +2207,11 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A58" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -2466,15 +2238,11 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A59" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B59" t="n">
+        <v>5</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -2501,15 +2269,11 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A60" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -2536,15 +2300,11 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A61" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B61" t="n">
+        <v>3</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2571,15 +2331,11 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A62" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B62" t="n">
+        <v>7</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2606,15 +2362,11 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A63" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B63" t="n">
+        <v>6</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -2641,15 +2393,11 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A64" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B64" t="n">
+        <v>4</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -2676,15 +2424,11 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A65" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B65" t="n">
+        <v>8</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -2711,15 +2455,11 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A66" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B66" t="n">
+        <v>4</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2746,15 +2486,11 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A67" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B67" t="n">
+        <v>6</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2781,15 +2517,11 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A68" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B68" t="n">
+        <v>2</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2816,15 +2548,11 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A69" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B69" t="n">
+        <v>3</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2851,15 +2579,11 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A70" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B70" t="n">
+        <v>7</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2886,15 +2610,11 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A71" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2921,15 +2641,11 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A72" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2956,15 +2672,11 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A73" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B73" t="n">
+        <v>8</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2991,15 +2703,11 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A74" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B74" t="n">
+        <v>7</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -3026,15 +2734,11 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A75" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B75" t="n">
+        <v>4</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -3061,15 +2765,11 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A76" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B76" t="n">
+        <v>2</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3096,15 +2796,11 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A77" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B77" t="n">
+        <v>8</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -3131,15 +2827,11 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A78" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B78" t="n">
+        <v>5</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -3166,15 +2858,11 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A79" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -3201,15 +2889,11 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A80" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B80" t="n">
+        <v>3</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -3236,15 +2920,11 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A81" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B81" t="n">
+        <v>6</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -3271,15 +2951,11 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A82" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B82" t="n">
+        <v>5</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -3306,15 +2982,11 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A83" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B83" t="n">
+        <v>6</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -3341,15 +3013,11 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A84" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B84" t="n">
+        <v>1</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -3376,15 +3044,11 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A85" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B85" t="n">
+        <v>4</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -3411,15 +3075,11 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A86" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B86" t="n">
+        <v>3</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -3446,15 +3106,11 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A87" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -3481,15 +3137,11 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A88" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B88" t="n">
+        <v>7</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -3516,15 +3168,11 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A89" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B89" t="n">
+        <v>8</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -3551,15 +3199,11 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A90" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B90" t="n">
+        <v>6</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -3586,15 +3230,11 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A91" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B91" t="n">
+        <v>7</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -3621,15 +3261,11 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A92" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B92" t="n">
+        <v>5</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -3656,15 +3292,11 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A93" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B93" t="n">
+        <v>8</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -3691,15 +3323,11 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A94" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B94" t="n">
+        <v>5</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -3726,15 +3354,11 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A95" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B95" t="n">
+        <v>7</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -3761,15 +3385,11 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A96" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -3796,15 +3416,11 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A97" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B97" t="n">
+        <v>8</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -3831,15 +3447,11 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A98" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B98" t="n">
+        <v>2</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -3866,15 +3478,11 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A99" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B99" t="n">
+        <v>3</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -3901,15 +3509,11 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A100" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B100" t="n">
+        <v>6</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -3936,15 +3540,11 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A101" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B101" t="n">
+        <v>4</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -3971,15 +3571,11 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A102" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B102" t="n">
+        <v>3</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -4006,15 +3602,11 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A103" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B103" t="n">
+        <v>4</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -4041,15 +3633,11 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A104" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B104" t="n">
+        <v>5</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -4076,15 +3664,11 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A105" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B105" t="n">
+        <v>2</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -4111,15 +3695,11 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A106" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B106" t="n">
+        <v>6</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -4146,15 +3726,11 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A107" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B107" t="n">
+        <v>7</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -4181,15 +3757,11 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A108" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B108" t="n">
+        <v>1</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -4216,15 +3788,11 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A109" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B109" t="n">
+        <v>8</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -4251,15 +3819,11 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
+      <c r="A110" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B110" t="n">
+        <v>8</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -4286,15 +3850,11 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
+      <c r="A111" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B111" t="n">
+        <v>1</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -4321,15 +3881,11 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
+      <c r="A112" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B112" t="n">
+        <v>6</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -4356,15 +3912,11 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
+      <c r="A113" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B113" t="n">
+        <v>5</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -4391,15 +3943,11 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
+      <c r="A114" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B114" t="n">
+        <v>4</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -4426,15 +3974,11 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
+      <c r="A115" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B115" t="n">
+        <v>3</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -4461,15 +4005,11 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+      <c r="A116" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B116" t="n">
+        <v>7</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -4496,15 +4036,11 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
+      <c r="A117" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B117" t="n">
+        <v>2</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>

</xml_diff>